<commit_message>
added react testing files, changed html icon
</commit_message>
<xml_diff>
--- a/project_management/timeline.xlsx
+++ b/project_management/timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285878B0-5890-4823-9DE6-9C986297754C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A238A1-24E9-4A1B-B666-589DA015984E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F7264979-8943-4592-AFFE-E5581CAB8C55}"/>
   </bookViews>
@@ -474,8 +474,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3300"/>
       <color rgb="FFFF6600"/>
-      <color rgb="FFFF3300"/>
       <color rgb="FFFFFFFF"/>
       <color rgb="FFFFE41D"/>
       <color rgb="FFFF0066"/>
@@ -4359,7 +4359,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF6600"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </c:spPr>
             <c:extLst>
@@ -4374,7 +4374,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF6600"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </c:spPr>
             <c:extLst>
@@ -4389,7 +4389,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF6600"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </c:spPr>
             <c:extLst>
@@ -4440,6 +4440,21 @@
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000029-BFAD-45CB-95E7-7B2794EA571B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF3300"/>
+              </a:solidFill>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000030-9739-46E6-9D04-4795973E77DF}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -20723,7 +20738,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated template for standup and formatting of sprint3_standups.md
</commit_message>
<xml_diff>
--- a/project_management/timeline.xlsx
+++ b/project_management/timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A238A1-24E9-4A1B-B666-589DA015984E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641D7835-05BE-4932-86FF-D7DDFCDC721B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F7264979-8943-4592-AFFE-E5581CAB8C55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F7264979-8943-4592-AFFE-E5581CAB8C55}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -373,6 +373,15 @@
   <si>
     <t>Delete row</t>
   </si>
+  <si>
+    <t>Documentation Catchup</t>
+  </si>
+  <si>
+    <t>Retro3: Reward System 2.0</t>
+  </si>
+  <si>
+    <t>Intro to Code Reviews &amp; Testing</t>
+  </si>
 </sst>
 </file>
 
@@ -597,9 +606,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Rough!$B$2:$B$13</c:f>
+              <c:f>Rough!$B$2:$B$15</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Project Setup</c:v>
                 </c:pt>
@@ -616,21 +625,30 @@
                   <c:v>Data Entry Table</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Database Setup &amp; Integration</c:v>
+                  <c:v>Documentation Catchup</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Backend Setup</c:v>
+                  <c:v>Retro3: Reward System 2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Intro to Code Reviews &amp; Testing</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Stat Card System</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Notion API Integration</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Feedback System</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Database Setup &amp; Integration</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Backend Setup</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Notion API Integration</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Time Estimation Autofill</c:v>
                 </c:pt>
               </c:strCache>
@@ -638,10 +656,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Rough!$D$2:$D$12</c:f>
+              <c:f>Rough!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>45787</c:v>
                 </c:pt>
@@ -657,23 +675,32 @@
                 <c:pt idx="4">
                   <c:v>45809</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="5" formatCode="d\-mmm">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="6" formatCode="d\-mmm">
+                  <c:v>45819</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="d\-mmm">
                   <c:v>45820</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>45827</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>45824</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="d\-mmm">
                   <c:v>45829</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="d\-mmm">
-                  <c:v>45832</c:v>
-                </c:pt>
                 <c:pt idx="10" formatCode="d\-mmm">
-                  <c:v>45838</c:v>
+                  <c:v>45833</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45836</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45840</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="d\-mmm">
+                  <c:v>45842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -714,7 +741,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -733,7 +760,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -752,7 +779,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -766,12 +793,31 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-2A32-4777-86FB-06FB9168A116}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="4"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -790,6 +836,89 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-0AEE-4D0C-B25B-5F630A6806E3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-0AEE-4D0C-B25B-5F630A6806E3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-0AEE-4D0C-B25B-5F630A6806E3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-0AEE-4D0C-B25B-5F630A6806E3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:ln>
@@ -797,52 +926,9 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-0AEE-4D0C-B25B-5F630A6806E3}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000A-0AEE-4D0C-B25B-5F630A6806E3}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-0AEE-4D0C-B25B-5F630A6806E3}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -854,36 +940,9 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000C-0AEE-4D0C-B25B-5F630A6806E3}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-0AEE-4D0C-B25B-5F630A6806E3}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -895,17 +954,12 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000E-0AEE-4D0C-B25B-5F630A6806E3}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Rough!$B$2:$B$13</c:f>
+              <c:f>Rough!$B$2:$B$15</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Project Setup</c:v>
                 </c:pt>
@@ -922,21 +976,30 @@
                   <c:v>Data Entry Table</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Database Setup &amp; Integration</c:v>
+                  <c:v>Documentation Catchup</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Backend Setup</c:v>
+                  <c:v>Retro3: Reward System 2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Intro to Code Reviews &amp; Testing</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Stat Card System</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Notion API Integration</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Feedback System</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Database Setup &amp; Integration</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Backend Setup</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Notion API Integration</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Time Estimation Autofill</c:v>
                 </c:pt>
               </c:strCache>
@@ -944,10 +1007,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Rough!$F$2:$F$12</c:f>
+              <c:f>Rough!$F$2:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -964,22 +1027,31 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1014,12 +1086,62 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Rough!$B$2:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>Project Setup</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Intro to Solo-scrum</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>UI/UX Foundation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Intro to React</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Data Entry Table</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Documentation Catchup</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Retro3: Reward System 2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Intro to Code Reviews &amp; Testing</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Stat Card System</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Feedback System</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Database Setup &amp; Integration</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Backend Setup</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Notion API Integration</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Time Estimation Autofill</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Rough!$C$2:$C$12</c:f>
+              <c:f>Rough!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1112,7 +1234,7 @@
         <c:axId val="523900576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45841"/>
+          <c:max val="45844"/>
           <c:min val="45787"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1318,9 +1440,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Rough!$B$2:$B$13</c:f>
+              <c:f>Rough!$B$2:$B$9</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Project Setup</c:v>
                 </c:pt>
@@ -1337,32 +1459,23 @@
                   <c:v>Data Entry Table</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Database Setup &amp; Integration</c:v>
+                  <c:v>Documentation Catchup</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Backend Setup</c:v>
+                  <c:v>Retro3: Reward System 2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Stat Card System</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Notion API Integration</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Feedback System</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Time Estimation Autofill</c:v>
+                  <c:v>Intro to Code Reviews &amp; Testing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Rough!$D$2:$D$12</c:f>
+              <c:f>Rough!$D$2:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>45787</c:v>
                 </c:pt>
@@ -1378,23 +1491,32 @@
                 <c:pt idx="4">
                   <c:v>45809</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="5" formatCode="d\-mmm">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="6" formatCode="d\-mmm">
+                  <c:v>45819</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="d\-mmm">
                   <c:v>45820</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>45827</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>45824</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="d\-mmm">
                   <c:v>45829</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="d\-mmm">
-                  <c:v>45832</c:v>
-                </c:pt>
                 <c:pt idx="10" formatCode="d\-mmm">
-                  <c:v>45838</c:v>
+                  <c:v>45833</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45836</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45840</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="d\-mmm">
+                  <c:v>45842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1525,69 +1647,12 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="5"/>
+            <c:idx val="8"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000A-0EFA-41F7-B770-1FAF1E140739}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000C-0EFA-41F7-B770-1FAF1E140739}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000E-0EFA-41F7-B770-1FAF1E140739}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF5050"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1628,6 +1693,53 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-0EFA-41F7-B770-1FAF1E140739}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF5050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
               </a:solidFill>
               <a:ln>
@@ -1635,17 +1747,12 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000014-0EFA-41F7-B770-1FAF1E140739}"/>
-              </c:ext>
-            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Rough!$B$2:$B$13</c:f>
+              <c:f>Rough!$B$2:$B$9</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Project Setup</c:v>
                 </c:pt>
@@ -1662,32 +1769,23 @@
                   <c:v>Data Entry Table</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Database Setup &amp; Integration</c:v>
+                  <c:v>Documentation Catchup</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Backend Setup</c:v>
+                  <c:v>Retro3: Reward System 2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Stat Card System</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Notion API Integration</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Feedback System</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Time Estimation Autofill</c:v>
+                  <c:v>Intro to Code Reviews &amp; Testing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Rough!$F$2:$F$12</c:f>
+              <c:f>Rough!$F$2:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -1704,22 +1802,31 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1756,10 +1863,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Rough!$C$2:$C$12</c:f>
+              <c:f>Rough!$C$2:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -18977,16 +19084,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>257163</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>90783</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>188582</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>45063</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>88789</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>3974</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>388619</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>141134</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20463,8 +20570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5AF2C9-7080-46F5-B693-88D30594D7FD}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20531,13 +20638,13 @@
         <v>45797</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F12" si="0">E3-D3</f>
+        <f t="shared" ref="F3:F9" si="0">E3-D3</f>
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A12" si="1">A3+1</f>
+        <f t="shared" ref="A4:A15" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -20607,17 +20714,17 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5">
+        <v>111</v>
+      </c>
+      <c r="D7" s="1">
         <v>45817</v>
       </c>
       <c r="E7" s="1">
-        <v>45820</v>
+        <v>45819</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -20626,17 +20733,17 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="5">
-        <v>45820</v>
+        <v>112</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45819</v>
       </c>
       <c r="E8" s="1">
-        <v>45827</v>
+        <v>45824</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -20645,17 +20752,17 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="5">
-        <v>45827</v>
+        <v>113</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45820</v>
       </c>
       <c r="E9" s="1">
-        <v>45829</v>
+        <v>45824</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -20664,17 +20771,17 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D10" s="5">
+        <v>45824</v>
+      </c>
+      <c r="E10" s="1">
         <v>45829</v>
       </c>
-      <c r="E10" s="1">
-        <v>45832</v>
-      </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>E10-D10</f>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -20686,14 +20793,14 @@
         <v>17</v>
       </c>
       <c r="D11" s="1">
-        <v>45832</v>
+        <v>45829</v>
       </c>
       <c r="E11" s="1">
-        <v>45838</v>
+        <v>45833</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>E11-D11</f>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -20702,30 +20809,75 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1">
-        <v>45838</v>
+        <v>45833</v>
       </c>
       <c r="E12" s="1">
-        <v>45841</v>
+        <v>45836</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f>E12-D12</f>
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5">
+        <v>45836</v>
+      </c>
+      <c r="E13" s="1">
+        <v>45840</v>
+      </c>
+      <c r="F13">
+        <f>E13-D13</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="5"/>
-      <c r="E14" s="1"/>
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45840</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45842</v>
+      </c>
+      <c r="F14">
+        <f>E14-D14</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="5"/>
-      <c r="E15" s="1"/>
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45842</v>
+      </c>
+      <c r="E15" s="1">
+        <v>45844</v>
+      </c>
+      <c r="F15">
+        <f>E15-D15</f>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20737,7 +20889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63633C4B-C2B0-414D-AE3B-54E8394185B5}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added back testing files, made some documentation changes
</commit_message>
<xml_diff>
--- a/project_management/timeline.xlsx
+++ b/project_management/timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B6F3FE-023C-41E2-9F75-B2B5C4FF97E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7336D336-6201-48E4-90BA-F28EB2DFB89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F7264979-8943-4592-AFFE-E5581CAB8C55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{F7264979-8943-4592-AFFE-E5581CAB8C55}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -24805,8 +24805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BEF2CE-DB08-45F6-BBD9-08B42BE384C3}">
   <dimension ref="A1:AE58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25587,7 +25587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72305F46-33BC-4086-BBC4-63DE2AF7FDE2}">
   <dimension ref="B10:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:E25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
handled synch issues with backend_setup branch src/backend folder
</commit_message>
<xml_diff>
--- a/project_management/timeline.xlsx
+++ b/project_management/timeline.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7336D336-6201-48E4-90BA-F28EB2DFB89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BA3F99-8F49-4D05-B6ED-D7D3237BDB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{F7264979-8943-4592-AFFE-E5581CAB8C55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F7264979-8943-4592-AFFE-E5581CAB8C55}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="Rough" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 3" sheetId="5" r:id="rId3"/>
     <sheet name="Sprint 4" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
+    <sheet name="Sprint 6" sheetId="8" r:id="rId5"/>
     <sheet name="(Old) Sprint2-3" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="166">
   <si>
     <t>ID</t>
   </si>
@@ -645,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -667,7 +667,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -677,8 +676,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9900"/>
       <color rgb="FF99FF33"/>
-      <color rgb="FFFF9900"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF3366CC"/>
       <color rgb="FF9966FF"/>
@@ -804,7 +803,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Rough!$B$2:$B$15</c:f>
+              <c:f>Rough!$B$2:$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -835,13 +834,13 @@
                   <c:v>Stat Card System</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>Database Setup &amp; Integration</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Backend Setup</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Feedback System</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Database Setup &amp; Integration</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Backend Setup</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Notion API Integration</c:v>
@@ -886,19 +885,19 @@
                   <c:v>45824</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="d\-mmm">
-                  <c:v>45829</c:v>
+                  <c:v>45832</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="d\-mmm">
-                  <c:v>45833</c:v>
+                  <c:v>45832</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45836</c:v>
+                  <c:v>45839</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45840</c:v>
+                  <c:v>45845</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="d\-mmm">
-                  <c:v>45842</c:v>
+                  <c:v>45848</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1201,7 +1200,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Rough!$B$2:$B$15</c:f>
+              <c:f>Rough!$B$2:$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1232,13 +1231,13 @@
                   <c:v>Stat Card System</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>Database Setup &amp; Integration</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Backend Setup</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Feedback System</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Database Setup &amp; Integration</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Backend Setup</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Notion API Integration</c:v>
@@ -1280,22 +1279,22 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1332,7 +1331,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Rough!$B$2:$B$15</c:f>
+              <c:f>Rough!$B$2:$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1363,13 +1362,13 @@
                   <c:v>Stat Card System</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>Database Setup &amp; Integration</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Backend Setup</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Feedback System</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Database Setup &amp; Integration</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Backend Setup</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Notion API Integration</c:v>
@@ -1470,7 +1469,7 @@
         <c:axId val="523900576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45844"/>
+          <c:max val="45852"/>
           <c:min val="45787"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1577,727 +1576,6 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Timeline: Sprints 2 Backlogs &amp; Subtasks</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'(Old) Sprint2-3'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Start_Date</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'(Old) Sprint2-3'!$C$2:$C$13</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Edit SDP: detailed timeline for sprints 2 &amp; 3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Populate web app with static components</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Complete 2nd, more difficult quiz with 75% or greater</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Add button to append new page to table</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Enable cell-click updates</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Add calendar for start/end date columns</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Restrict numeric column to positive inputs</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Implement dropdown for categories</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Load category names/colors from text file</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Add time summation feature</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Add row deletion feature via mouse selection</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Write unit tests</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'(Old) Sprint2-3'!$D$2:$D$13</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>45797</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45798</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45800</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45798</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45798</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45799</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45799</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45800</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45800</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45801</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>45801</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>45801</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-070E-4BA7-97FA-B70CBFE535C1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'(Old) Sprint2-3'!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Duration</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0066"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000008-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000A-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000C-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="11"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-070E-4BA7-97FA-B70CBFE535C1}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:cat>
-            <c:strRef>
-              <c:f>'(Old) Sprint2-3'!$C$2:$C$13</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Edit SDP: detailed timeline for sprints 2 &amp; 3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Populate web app with static components</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Complete 2nd, more difficult quiz with 75% or greater</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Add button to append new page to table</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Enable cell-click updates</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Add calendar for start/end date columns</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Restrict numeric column to positive inputs</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Implement dropdown for categories</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Load category names/colors from text file</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Add time summation feature</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Add row deletion feature via mouse selection</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Write unit tests</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'(Old) Sprint2-3'!$F$2:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-070E-4BA7-97FA-B70CBFE535C1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="1620074624"/>
-        <c:axId val="1620076064"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1620074624"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1620076064"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1620076064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="45802"/>
-          <c:min val="45797"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="t"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="[$-409]d\-mmm;@" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1620074624"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9147,632 +8425,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$D$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Start_Date</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet2!$B$11:$C$25</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="15"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Create sprint 4 timeline</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Update mvs</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Write up new plan document</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Design templates</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Implement plan</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Upload plan results page</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Setup</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Research Vitest + React testing-library</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Unit Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Integration testing</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Pull Request</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Leave comments</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Update code</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Changes documentation</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Merge with main</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Documentation Catchup</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Documentation Catchup</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Retro3: Reward System 2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Retro3: Reward System 2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Retro3: Reward System 2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Retro3: Reward System 2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$D$11:$D$25</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>45820</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45820</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45820</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45820</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45821</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45829</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45820</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45821</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45821</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45822</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>45823</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>45823</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>45824</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>45826</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>45827</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A587-428F-9798-1A0D6AA927FB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$E$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Duration</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet2!$B$11:$C$25</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="15"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Create sprint 4 timeline</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Update mvs</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Write up new plan document</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Design templates</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Implement plan</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Upload plan results page</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Setup</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Research Vitest + React testing-library</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Unit Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Integration testing</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Pull Request</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Leave comments</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Update code</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Changes documentation</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Merge with main</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Documentation Catchup</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Documentation Catchup</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Retro3: Reward System 2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Retro3: Reward System 2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Retro3: Reward System 2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Retro3: Reward System 2.0</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>Intro to Code Reviews &amp; Testing</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$E$11:$E$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A587-428F-9798-1A0D6AA927FB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="2057150288"/>
-        <c:axId val="2057150768"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2057150288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2057150768"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2057150768"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2057150288"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -17446,7 +16098,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -18117,6 +16769,727 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1765708624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Timeline: Sprints 2 Backlogs &amp; Subtasks</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'(Old) Sprint2-3'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start_Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'(Old) Sprint2-3'!$C$2:$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Edit SDP: detailed timeline for sprints 2 &amp; 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Populate web app with static components</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Complete 2nd, more difficult quiz with 75% or greater</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Add button to append new page to table</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Enable cell-click updates</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Add calendar for start/end date columns</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Restrict numeric column to positive inputs</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Implement dropdown for categories</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Load category names/colors from text file</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Add time summation feature</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Add row deletion feature via mouse selection</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Write unit tests</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'(Old) Sprint2-3'!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>45797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45798</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45799</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45799</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45801</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45801</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-070E-4BA7-97FA-B70CBFE535C1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'(Old) Sprint2-3'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0066"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-070E-4BA7-97FA-B70CBFE535C1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'(Old) Sprint2-3'!$C$2:$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Edit SDP: detailed timeline for sprints 2 &amp; 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Populate web app with static components</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Complete 2nd, more difficult quiz with 75% or greater</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Add button to append new page to table</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Enable cell-click updates</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Add calendar for start/end date columns</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Restrict numeric column to positive inputs</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Implement dropdown for categories</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Load category names/colors from text file</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Add time summation feature</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Add row deletion feature via mouse selection</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Write unit tests</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'(Old) Sprint2-3'!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-070E-4BA7-97FA-B70CBFE535C1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1620074624"/>
+        <c:axId val="1620076064"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1620074624"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1620076064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1620076064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="45802"/>
+          <c:min val="45797"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="[$-409]d\-mmm;@" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1620074624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18373,46 +17746,6 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -21482,525 +20815,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>512457</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>96071</xdr:rowOff>
+      <xdr:colOff>474357</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>65591</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22025,6 +20853,333 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89CD654C-F594-5012-D728-C44A07C059BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10088880" y="1684020"/>
+          <a:ext cx="563880" cy="2979420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF9900">
+            <a:alpha val="50000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Isosceles Triangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6770914-A61E-1C8A-165B-D01837791999}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="10203180" y="3360420"/>
+          <a:ext cx="312420" cy="213360"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E23FE063-1BFC-0CF5-D54D-ED10FE6B4BB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10050780" y="2019300"/>
+          <a:ext cx="640080" cy="434340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Sprint 6</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>6/24-29</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20ACDFC1-E3CF-4727-BA0E-B21A1AC00236}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10096500" y="2880360"/>
+          <a:ext cx="571500" cy="434340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Today</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>6/28</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -22759,47 +21914,6 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C52C763F-C8F5-BC8B-D4C5-2C2DCAFEAAB9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -24093,8 +23207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5AF2C9-7080-46F5-B693-88D30594D7FD}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24300,11 +23414,11 @@
         <v>45824</v>
       </c>
       <c r="E10" s="1">
-        <v>45829</v>
+        <v>45831</v>
       </c>
       <c r="F10">
         <f t="shared" ref="F10:F15" si="2">E10-D10</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -24313,17 +23427,17 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1">
-        <v>45829</v>
+        <v>45832</v>
       </c>
       <c r="E11" s="1">
-        <v>45833</v>
+        <v>45839</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -24332,17 +23446,17 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1">
-        <v>45833</v>
+        <v>45832</v>
       </c>
       <c r="E12" s="1">
-        <v>45836</v>
+        <v>45839</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -24351,17 +23465,17 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" s="5">
-        <v>45836</v>
+        <v>45839</v>
       </c>
       <c r="E13" s="1">
-        <v>45840</v>
+        <v>45845</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -24373,14 +23487,14 @@
         <v>13</v>
       </c>
       <c r="D14" s="5">
-        <v>45840</v>
+        <v>45845</v>
       </c>
       <c r="E14" s="1">
-        <v>45842</v>
+        <v>45848</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -24392,14 +23506,14 @@
         <v>18</v>
       </c>
       <c r="D15" s="1">
-        <v>45842</v>
+        <v>45848</v>
       </c>
       <c r="E15" s="1">
-        <v>45844</v>
+        <v>45852</v>
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -24412,7 +23526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63633C4B-C2B0-414D-AE3B-54E8394185B5}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -24805,7 +23919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BEF2CE-DB08-45F6-BBD9-08B42BE384C3}">
   <dimension ref="A1:AE58"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23:G33"/>
     </sheetView>
   </sheetViews>
@@ -25349,233 +24463,233 @@
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W37" s="22"/>
-      <c r="X37" s="22"/>
-      <c r="Y37" s="22"/>
-      <c r="Z37" s="22"/>
-      <c r="AA37" s="22"/>
-      <c r="AB37" s="22"/>
-      <c r="AC37" s="22"/>
-      <c r="AD37" s="22"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="21"/>
+      <c r="Z37" s="21"/>
+      <c r="AA37" s="21"/>
+      <c r="AB37" s="21"/>
+      <c r="AC37" s="21"/>
+      <c r="AD37" s="21"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W38" s="22"/>
-      <c r="X38" s="22"/>
-      <c r="Y38" s="22"/>
-      <c r="Z38" s="22"/>
-      <c r="AA38" s="22"/>
-      <c r="AB38" s="22"/>
-      <c r="AC38" s="22"/>
-      <c r="AD38" s="22"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="21"/>
+      <c r="Z38" s="21"/>
+      <c r="AA38" s="21"/>
+      <c r="AB38" s="21"/>
+      <c r="AC38" s="21"/>
+      <c r="AD38" s="21"/>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W39" s="22"/>
-      <c r="X39" s="22"/>
-      <c r="Y39" s="22"/>
-      <c r="Z39" s="22"/>
-      <c r="AA39" s="22"/>
-      <c r="AB39" s="22"/>
-      <c r="AC39" s="22"/>
-      <c r="AD39" s="22"/>
+      <c r="W39" s="21"/>
+      <c r="X39" s="21"/>
+      <c r="Y39" s="21"/>
+      <c r="Z39" s="21"/>
+      <c r="AA39" s="21"/>
+      <c r="AB39" s="21"/>
+      <c r="AC39" s="21"/>
+      <c r="AD39" s="21"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W40" s="22"/>
-      <c r="X40" s="22"/>
-      <c r="Y40" s="22"/>
-      <c r="Z40" s="22"/>
-      <c r="AA40" s="22"/>
-      <c r="AB40" s="22"/>
-      <c r="AC40" s="22"/>
-      <c r="AD40" s="22"/>
+      <c r="W40" s="21"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="21"/>
+      <c r="Z40" s="21"/>
+      <c r="AA40" s="21"/>
+      <c r="AB40" s="21"/>
+      <c r="AC40" s="21"/>
+      <c r="AD40" s="21"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W41" s="22"/>
-      <c r="X41" s="22"/>
-      <c r="Y41" s="22"/>
-      <c r="Z41" s="22"/>
-      <c r="AA41" s="22"/>
-      <c r="AB41" s="22"/>
-      <c r="AC41" s="22"/>
-      <c r="AD41" s="22"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
+      <c r="Z41" s="21"/>
+      <c r="AA41" s="21"/>
+      <c r="AB41" s="21"/>
+      <c r="AC41" s="21"/>
+      <c r="AD41" s="21"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W42" s="22"/>
-      <c r="X42" s="22"/>
-      <c r="Y42" s="22"/>
-      <c r="Z42" s="22"/>
-      <c r="AA42" s="22"/>
-      <c r="AB42" s="22"/>
-      <c r="AC42" s="22"/>
-      <c r="AD42" s="22"/>
+      <c r="W42" s="21"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="21"/>
+      <c r="Z42" s="21"/>
+      <c r="AA42" s="21"/>
+      <c r="AB42" s="21"/>
+      <c r="AC42" s="21"/>
+      <c r="AD42" s="21"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W43" s="22"/>
-      <c r="X43" s="22"/>
-      <c r="Y43" s="22"/>
-      <c r="Z43" s="22"/>
-      <c r="AA43" s="22"/>
-      <c r="AB43" s="22"/>
-      <c r="AC43" s="22"/>
-      <c r="AD43" s="22"/>
+      <c r="W43" s="21"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="21"/>
+      <c r="Z43" s="21"/>
+      <c r="AA43" s="21"/>
+      <c r="AB43" s="21"/>
+      <c r="AC43" s="21"/>
+      <c r="AD43" s="21"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W44" s="22"/>
-      <c r="X44" s="22"/>
-      <c r="Y44" s="22"/>
-      <c r="Z44" s="22"/>
-      <c r="AA44" s="22"/>
-      <c r="AB44" s="22"/>
-      <c r="AC44" s="22"/>
-      <c r="AD44" s="22"/>
+      <c r="W44" s="21"/>
+      <c r="X44" s="21"/>
+      <c r="Y44" s="21"/>
+      <c r="Z44" s="21"/>
+      <c r="AA44" s="21"/>
+      <c r="AB44" s="21"/>
+      <c r="AC44" s="21"/>
+      <c r="AD44" s="21"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W45" s="22"/>
-      <c r="X45" s="22"/>
-      <c r="Y45" s="22"/>
-      <c r="Z45" s="22"/>
-      <c r="AA45" s="22"/>
-      <c r="AB45" s="22"/>
-      <c r="AC45" s="22"/>
-      <c r="AD45" s="22"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="21"/>
+      <c r="Z45" s="21"/>
+      <c r="AA45" s="21"/>
+      <c r="AB45" s="21"/>
+      <c r="AC45" s="21"/>
+      <c r="AD45" s="21"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W46" s="22"/>
-      <c r="X46" s="22"/>
-      <c r="Y46" s="22"/>
-      <c r="Z46" s="22"/>
-      <c r="AA46" s="22"/>
-      <c r="AB46" s="22"/>
-      <c r="AC46" s="22"/>
-      <c r="AD46" s="22"/>
+      <c r="W46" s="21"/>
+      <c r="X46" s="21"/>
+      <c r="Y46" s="21"/>
+      <c r="Z46" s="21"/>
+      <c r="AA46" s="21"/>
+      <c r="AB46" s="21"/>
+      <c r="AC46" s="21"/>
+      <c r="AD46" s="21"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W47" s="22"/>
-      <c r="X47" s="22"/>
-      <c r="Y47" s="22"/>
-      <c r="Z47" s="22"/>
-      <c r="AA47" s="22"/>
-      <c r="AB47" s="22"/>
-      <c r="AC47" s="22"/>
-      <c r="AD47" s="22"/>
+      <c r="W47" s="21"/>
+      <c r="X47" s="21"/>
+      <c r="Y47" s="21"/>
+      <c r="Z47" s="21"/>
+      <c r="AA47" s="21"/>
+      <c r="AB47" s="21"/>
+      <c r="AC47" s="21"/>
+      <c r="AD47" s="21"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="W48" s="22"/>
-      <c r="X48" s="22"/>
-      <c r="Y48" s="22"/>
-      <c r="Z48" s="22"/>
-      <c r="AA48" s="22"/>
-      <c r="AB48" s="22"/>
-      <c r="AC48" s="22"/>
-      <c r="AD48" s="22"/>
+      <c r="W48" s="21"/>
+      <c r="X48" s="21"/>
+      <c r="Y48" s="21"/>
+      <c r="Z48" s="21"/>
+      <c r="AA48" s="21"/>
+      <c r="AB48" s="21"/>
+      <c r="AC48" s="21"/>
+      <c r="AD48" s="21"/>
     </row>
     <row r="49" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W49" s="22"/>
-      <c r="X49" s="22"/>
-      <c r="Y49" s="22"/>
-      <c r="Z49" s="22"/>
-      <c r="AA49" s="22"/>
-      <c r="AB49" s="22"/>
-      <c r="AC49" s="22"/>
-      <c r="AD49" s="22"/>
+      <c r="W49" s="21"/>
+      <c r="X49" s="21"/>
+      <c r="Y49" s="21"/>
+      <c r="Z49" s="21"/>
+      <c r="AA49" s="21"/>
+      <c r="AB49" s="21"/>
+      <c r="AC49" s="21"/>
+      <c r="AD49" s="21"/>
     </row>
     <row r="50" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W50" s="22"/>
-      <c r="X50" s="22"/>
-      <c r="Y50" s="22"/>
-      <c r="Z50" s="22"/>
-      <c r="AA50" s="22"/>
-      <c r="AB50" s="22"/>
-      <c r="AC50" s="22"/>
-      <c r="AD50" s="22"/>
-      <c r="AE50" s="22"/>
+      <c r="W50" s="21"/>
+      <c r="X50" s="21"/>
+      <c r="Y50" s="21"/>
+      <c r="Z50" s="21"/>
+      <c r="AA50" s="21"/>
+      <c r="AB50" s="21"/>
+      <c r="AC50" s="21"/>
+      <c r="AD50" s="21"/>
+      <c r="AE50" s="21"/>
     </row>
     <row r="51" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W51" s="22"/>
-      <c r="X51" s="22"/>
-      <c r="Y51" s="22"/>
-      <c r="Z51" s="22"/>
-      <c r="AA51" s="22"/>
-      <c r="AB51" s="22"/>
-      <c r="AC51" s="22"/>
-      <c r="AD51" s="22"/>
-      <c r="AE51" s="22"/>
+      <c r="W51" s="21"/>
+      <c r="X51" s="21"/>
+      <c r="Y51" s="21"/>
+      <c r="Z51" s="21"/>
+      <c r="AA51" s="21"/>
+      <c r="AB51" s="21"/>
+      <c r="AC51" s="21"/>
+      <c r="AD51" s="21"/>
+      <c r="AE51" s="21"/>
     </row>
     <row r="52" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W52" s="22"/>
-      <c r="X52" s="22"/>
-      <c r="Y52" s="22"/>
-      <c r="Z52" s="22"/>
-      <c r="AA52" s="22"/>
-      <c r="AB52" s="22"/>
-      <c r="AC52" s="22"/>
-      <c r="AD52" s="22"/>
-      <c r="AE52" s="22"/>
+      <c r="W52" s="21"/>
+      <c r="X52" s="21"/>
+      <c r="Y52" s="21"/>
+      <c r="Z52" s="21"/>
+      <c r="AA52" s="21"/>
+      <c r="AB52" s="21"/>
+      <c r="AC52" s="21"/>
+      <c r="AD52" s="21"/>
+      <c r="AE52" s="21"/>
     </row>
     <row r="53" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W53" s="22"/>
-      <c r="X53" s="22"/>
-      <c r="Y53" s="22"/>
-      <c r="Z53" s="22"/>
-      <c r="AA53" s="22"/>
-      <c r="AB53" s="22"/>
-      <c r="AC53" s="22"/>
-      <c r="AD53" s="22"/>
-      <c r="AE53" s="22"/>
+      <c r="W53" s="21"/>
+      <c r="X53" s="21"/>
+      <c r="Y53" s="21"/>
+      <c r="Z53" s="21"/>
+      <c r="AA53" s="21"/>
+      <c r="AB53" s="21"/>
+      <c r="AC53" s="21"/>
+      <c r="AD53" s="21"/>
+      <c r="AE53" s="21"/>
     </row>
     <row r="54" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W54" s="22"/>
-      <c r="X54" s="22"/>
-      <c r="Y54" s="22"/>
-      <c r="Z54" s="22"/>
-      <c r="AA54" s="22"/>
-      <c r="AB54" s="22"/>
-      <c r="AC54" s="22"/>
-      <c r="AD54" s="22"/>
-      <c r="AE54" s="22"/>
+      <c r="W54" s="21"/>
+      <c r="X54" s="21"/>
+      <c r="Y54" s="21"/>
+      <c r="Z54" s="21"/>
+      <c r="AA54" s="21"/>
+      <c r="AB54" s="21"/>
+      <c r="AC54" s="21"/>
+      <c r="AD54" s="21"/>
+      <c r="AE54" s="21"/>
     </row>
     <row r="55" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W55" s="22"/>
-      <c r="X55" s="22"/>
-      <c r="Y55" s="22"/>
-      <c r="Z55" s="22"/>
-      <c r="AA55" s="22"/>
-      <c r="AB55" s="22"/>
-      <c r="AC55" s="22"/>
-      <c r="AD55" s="22"/>
-      <c r="AE55" s="22"/>
+      <c r="W55" s="21"/>
+      <c r="X55" s="21"/>
+      <c r="Y55" s="21"/>
+      <c r="Z55" s="21"/>
+      <c r="AA55" s="21"/>
+      <c r="AB55" s="21"/>
+      <c r="AC55" s="21"/>
+      <c r="AD55" s="21"/>
+      <c r="AE55" s="21"/>
     </row>
     <row r="56" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W56" s="22"/>
-      <c r="X56" s="22"/>
-      <c r="Y56" s="22"/>
-      <c r="Z56" s="22"/>
-      <c r="AA56" s="22"/>
-      <c r="AB56" s="22"/>
-      <c r="AC56" s="22"/>
-      <c r="AD56" s="22"/>
-      <c r="AE56" s="22"/>
+      <c r="W56" s="21"/>
+      <c r="X56" s="21"/>
+      <c r="Y56" s="21"/>
+      <c r="Z56" s="21"/>
+      <c r="AA56" s="21"/>
+      <c r="AB56" s="21"/>
+      <c r="AC56" s="21"/>
+      <c r="AD56" s="21"/>
+      <c r="AE56" s="21"/>
     </row>
     <row r="57" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W57" s="22"/>
-      <c r="X57" s="22"/>
-      <c r="Y57" s="22"/>
-      <c r="Z57" s="22"/>
-      <c r="AA57" s="22"/>
-      <c r="AB57" s="22"/>
-      <c r="AC57" s="22"/>
-      <c r="AD57" s="22"/>
-      <c r="AE57" s="22"/>
+      <c r="W57" s="21"/>
+      <c r="X57" s="21"/>
+      <c r="Y57" s="21"/>
+      <c r="Z57" s="21"/>
+      <c r="AA57" s="21"/>
+      <c r="AB57" s="21"/>
+      <c r="AC57" s="21"/>
+      <c r="AD57" s="21"/>
+      <c r="AE57" s="21"/>
     </row>
     <row r="58" spans="23:31" x14ac:dyDescent="0.3">
-      <c r="W58" s="22"/>
-      <c r="X58" s="22"/>
-      <c r="Y58" s="22"/>
-      <c r="Z58" s="22"/>
-      <c r="AA58" s="22"/>
-      <c r="AB58" s="22"/>
-      <c r="AC58" s="22"/>
-      <c r="AD58" s="22"/>
-      <c r="AE58" s="22"/>
+      <c r="W58" s="21"/>
+      <c r="X58" s="21"/>
+      <c r="Y58" s="21"/>
+      <c r="Z58" s="21"/>
+      <c r="AA58" s="21"/>
+      <c r="AB58" s="21"/>
+      <c r="AC58" s="21"/>
+      <c r="AD58" s="21"/>
+      <c r="AE58" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25584,242 +24698,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72305F46-33BC-4086-BBC4-63DE2AF7FDE2}">
-  <dimension ref="B10:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0181D7BC-7AD1-4D05-8552-EAE830B97C28}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" t="s">
-        <v>165</v>
-      </c>
-      <c r="D11" s="21">
-        <v>45820</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="21">
-        <v>45820</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="21">
-        <v>45820</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="21">
-        <v>45820</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" s="21">
-        <v>45821</v>
-      </c>
-      <c r="E15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="21">
-        <v>45829</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" s="21">
-        <v>45820</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D18" s="21">
-        <v>45821</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" s="21">
-        <v>45821</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="21">
-        <v>45822</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" s="21">
-        <v>45823</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" t="s">
-        <v>132</v>
-      </c>
-      <c r="D22" s="21">
-        <v>45823</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="21">
-        <v>45824</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" s="21">
-        <v>45826</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D25" s="21">
-        <v>45827</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added timeline + new standup log
</commit_message>
<xml_diff>
--- a/project_management/timeline.xlsx
+++ b/project_management/timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grego\Desktop\Coding\Projects\plan_tool\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5B71C9-6219-49AC-A060-D3B53D806C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2151319C-B372-4977-B47F-36A15ABB4F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F7264979-8943-4592-AFFE-E5581CAB8C55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F7264979-8943-4592-AFFE-E5581CAB8C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Rough" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="140">
   <si>
     <t>ID</t>
   </si>
@@ -455,6 +455,12 @@
   <si>
     <t>Backend Setup p1</t>
   </si>
+  <si>
+    <t>Plan Submission</t>
+  </si>
+  <si>
+    <t>Subsystem Integration</t>
+  </si>
 </sst>
 </file>
 
@@ -4581,13 +4587,13 @@
                   <c:v>Intro to Flask</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Frontend &amp; Backend Integration</c:v>
+                  <c:v>Subsystem Integration</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Feedback System</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Notion API Integration</c:v>
+                  <c:v>Plan Submission</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>End-to-End Testing</c:v>
@@ -4620,19 +4626,19 @@
                   <c:v>45901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45908</c:v>
+                  <c:v>45916</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45908</c:v>
+                  <c:v>45916</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45915</c:v>
+                  <c:v>45930</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45915</c:v>
+                  <c:v>45930</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45922</c:v>
+                  <c:v>45937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4858,13 +4864,13 @@
                   <c:v>Intro to Flask</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Frontend &amp; Backend Integration</c:v>
+                  <c:v>Subsystem Integration</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Feedback System</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Notion API Integration</c:v>
+                  <c:v>Plan Submission</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>End-to-End Testing</c:v>
@@ -4888,28 +4894,28 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4985,7 +4991,7 @@
         <c:axId val="1926341407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45927"/>
+          <c:max val="45943"/>
           <c:min val="45888"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -23421,13 +23427,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
+      <xdr:colOff>121920</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -23444,7 +23450,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10050780" y="2019300"/>
+          <a:off x="10073640" y="2019300"/>
           <a:ext cx="640080" cy="434340"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -23660,15 +23666,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23691,6 +23697,285 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1231C019-66FB-4B12-8766-083EB18BAF54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6880860" y="5173980"/>
+          <a:ext cx="1173480" cy="2217420"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67531BC6-72EB-DD7E-EBC8-E1B885E9FAC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7269480" y="5326380"/>
+          <a:ext cx="731520" cy="441960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Sprint 8 Sep</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> 1 - 16</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2179</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520339</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34FA89F7-EB9F-4ADB-9C7E-D50460E04F94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6969036" y="6560820"/>
+          <a:ext cx="518160" cy="446314"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Today</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>9/5</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>88177</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>423457</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Isosceles Triangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEB66E0A-97BA-77C4-421E-2CA46409308B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7055034" y="6266906"/>
+          <a:ext cx="335280" cy="248194"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -24894,7 +25179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5AF2C9-7080-46F5-B693-88D30594D7FD}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
@@ -25213,8 +25498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E16D282-9F0A-44F7-AD1B-719F64ACDC22}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25647,7 +25932,6 @@
         <v>45895</v>
       </c>
       <c r="E30">
-        <f t="shared" ref="E30:E32" si="3">D30-C30</f>
         <v>7</v>
       </c>
     </row>
@@ -25662,11 +25946,10 @@
         <v>45888</v>
       </c>
       <c r="D31" s="3">
-        <v>45895</v>
+        <v>45904</v>
       </c>
       <c r="E31">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -25680,11 +25963,10 @@
         <v>45888</v>
       </c>
       <c r="D32" s="3">
-        <v>45895</v>
+        <v>45904</v>
       </c>
       <c r="E32">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -25692,16 +25974,16 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C33" s="3">
         <v>45901</v>
       </c>
       <c r="D33" s="3">
-        <v>45906</v>
+        <v>45916</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -25712,13 +25994,13 @@
         <v>15</v>
       </c>
       <c r="C34" s="3">
-        <v>45908</v>
+        <v>45916</v>
       </c>
       <c r="D34" s="3">
-        <v>45913</v>
+        <v>45930</v>
       </c>
       <c r="E34">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -25726,16 +26008,16 @@
         <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="C35" s="3">
-        <v>45908</v>
+        <v>45916</v>
       </c>
       <c r="D35" s="3">
-        <v>45913</v>
+        <v>45930</v>
       </c>
       <c r="E35">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -25746,13 +26028,13 @@
         <v>131</v>
       </c>
       <c r="C36" s="3">
-        <v>45915</v>
+        <v>45930</v>
       </c>
       <c r="D36" s="3">
-        <v>45920</v>
+        <v>45937</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -25763,13 +26045,13 @@
         <v>132</v>
       </c>
       <c r="C37" s="3">
-        <v>45915</v>
+        <v>45930</v>
       </c>
       <c r="D37" s="3">
-        <v>45920</v>
+        <v>45937</v>
       </c>
       <c r="E37">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -25780,13 +26062,13 @@
         <v>133</v>
       </c>
       <c r="C38" s="3">
-        <v>45922</v>
+        <v>45937</v>
       </c>
       <c r="D38" s="3">
-        <v>45927</v>
+        <v>45943</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>